<commit_message>
240325 - finish REF tabular data
</commit_message>
<xml_diff>
--- a/UpdatedPracticeDemo_TabularData/Data/Config.xlsx
+++ b/UpdatedPracticeDemo_TabularData/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lanxess1-my.sharepoint.com/personal/hank_peng_ext_lanxess_com/Documents/Desktop/HanqinpGit_UiPath/UiPath/UpdatedPracticeDemo_TabularData/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\hanqinGIt\UiPath\UpdatedPracticeDemo_TabularData\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{CBBB4728-0F59-4619-B77C-39B7726D3910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1B0E1C0-06EF-438C-8654-B7BA3D6A983B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17BD613A-8922-45AD-A21E-8BB11A7A9F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -174,11 +174,18 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>C:\Users\Lvwcw\OneDrive - LANXESS Deutschland GmbH\Desktop\HanqinpGit_UiPath\UiPath\UpdatedPracticeDemo_TabularData\UiDemo-Crash\UiDemo.exe</t>
+    <t>data\Input\UiDemo-Transactions.xlsx</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>data\Input\UiDemo-Transactions.xlsx</t>
+    <t>C:\Users\Administrator\Desktop\hanqinGIt\UiPath\UpdatedPracticeDemo_TabularData\UiDemo-Crash\UiDemo.exe</t>
+  </si>
+  <si>
+    <t>StatusFilePath</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>data\Output\status.xlsx</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -243,7 +250,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -259,7 +266,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -558,15 +565,15 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
-    <col min="2" max="2" width="67.44140625" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="2" max="2" width="67.453125" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -603,7 +610,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -631,7 +638,7 @@
         <v>43</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>44</v>
@@ -643,7 +650,7 @@
         <v>45</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -656,7 +663,14 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1659,12 +1673,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1701,7 +1715,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1712,7 +1726,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1826,7 +1840,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -2825,12 +2839,12 @@
       <selection activeCell="B4" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.90625" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" customWidth="1"/>
+    <col min="3" max="3" width="60.36328125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>